<commit_message>
Finishted adjusting T5 pegasus testing and documentation.
</commit_message>
<xml_diff>
--- a/data/questions/QA.xlsx
+++ b/data/questions/QA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DVD\Desktop\MS project\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhysb\Git_Repositories\iTA\data\questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E79A34-ACE7-4D3A-A108-7EB519027DAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73BDCAFA-DC6C-4161-8F35-08A12132F010}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2D9F1CFF-57B0-48E4-8A67-9E1738541174}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2D9F1CFF-57B0-48E4-8A67-9E1738541174}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1624,14 +1624,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1949,272 +1948,272 @@
   <dimension ref="A1:B76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="86.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="86.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="109" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" ht="45">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" ht="30">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" ht="45">
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="45">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15">
+    <row r="6" spans="1:2" ht="29.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" ht="30">
       <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15">
+    <row r="10" spans="1:2" ht="29.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" ht="30">
       <c r="A11" t="s">
         <v>149</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15">
+    <row r="15" spans="1:2" ht="29.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>150</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15">
+    <row r="19" spans="1:2" ht="30">
       <c r="A19" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15">
+    <row r="20" spans="1:2" ht="29.25">
       <c r="A20" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>151</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15">
+    <row r="22" spans="1:2" ht="30">
       <c r="A22" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15">
+    <row r="23" spans="1:2" ht="29.25">
       <c r="A23" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15">
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15">
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15">
+    <row r="27" spans="1:2" ht="30">
       <c r="A27" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15">
+    <row r="28" spans="1:2" ht="29.25">
       <c r="A28" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15">
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15">
+    <row r="30" spans="1:2" ht="45">
       <c r="A30" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15">
+    <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15">
+    <row r="32" spans="1:2" ht="30">
       <c r="A32" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>61</v>
       </c>
@@ -2222,347 +2221,347 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15">
+    <row r="34" spans="1:2" ht="29.25">
       <c r="A34" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>65</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="15">
+    <row r="36" spans="1:2" ht="30">
       <c r="A36" t="s">
         <v>68</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15">
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>69</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="15">
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>71</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="15">
+    <row r="39" spans="1:2" ht="30">
       <c r="A39" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="15">
+    <row r="40" spans="1:2" ht="30">
       <c r="A40" t="s">
         <v>75</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="15">
+    <row r="41" spans="1:2">
       <c r="A41" t="s">
         <v>77</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="15">
+    <row r="42" spans="1:2">
       <c r="A42" t="s">
         <v>80</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="15">
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>81</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="15">
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>83</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="15">
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>85</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="15">
+    <row r="46" spans="1:2" ht="29.25">
       <c r="A46" t="s">
         <v>87</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="15">
+    <row r="47" spans="1:2" ht="30">
       <c r="A47" t="s">
         <v>89</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="15">
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>91</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="15">
+    <row r="49" spans="1:2" ht="30">
       <c r="A49" t="s">
         <v>93</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="15">
+    <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="15">
+    <row r="51" spans="1:2" ht="30">
       <c r="A51" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="15">
+    <row r="52" spans="1:2">
       <c r="A52" t="s">
         <v>98</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="15">
+    <row r="53" spans="1:2" ht="30">
       <c r="A53" t="s">
         <v>101</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="15">
+    <row r="54" spans="1:2" ht="30">
       <c r="A54" t="s">
         <v>103</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="15">
+    <row r="55" spans="1:2" ht="30">
       <c r="A55" t="s">
         <v>105</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="15">
+    <row r="56" spans="1:2">
       <c r="A56" t="s">
         <v>113</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" s="3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="15">
+    <row r="57" spans="1:2">
       <c r="A57" t="s">
         <v>114</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="15">
+    <row r="58" spans="1:2">
       <c r="A58" t="s">
         <v>115</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="15">
+    <row r="59" spans="1:2">
       <c r="A59" t="s">
         <v>116</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="15">
+    <row r="60" spans="1:2">
       <c r="A60" t="s">
         <v>117</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="15">
+    <row r="61" spans="1:2">
       <c r="A61" t="s">
         <v>118</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" s="3" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="15">
+    <row r="62" spans="1:2">
       <c r="A62" t="s">
         <v>107</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="15">
+    <row r="63" spans="1:2">
       <c r="A63" t="s">
         <v>108</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" s="3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="15">
+    <row r="64" spans="1:2">
       <c r="A64" t="s">
         <v>109</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B64" s="3" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="15">
+    <row r="65" spans="1:2" ht="30">
       <c r="A65" t="s">
         <v>110</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="15">
+    <row r="66" spans="1:2">
       <c r="A66" t="s">
         <v>111</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B66" s="3" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="15">
+    <row r="67" spans="1:2">
       <c r="A67" t="s">
         <v>112</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B67" s="3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="15">
+    <row r="68" spans="1:2" ht="30">
       <c r="A68" t="s">
         <v>131</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B68" s="3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="15">
+    <row r="69" spans="1:2">
       <c r="A69" t="s">
         <v>138</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B69" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="15">
+    <row r="70" spans="1:2" ht="45">
       <c r="A70" t="s">
         <v>139</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B70" s="3" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="15">
+    <row r="71" spans="1:2" ht="60">
       <c r="A71" t="s">
         <v>140</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B71" s="3" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="15">
+    <row r="72" spans="1:2" ht="75">
       <c r="A72" t="s">
         <v>141</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B72" s="3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="15">
+    <row r="73" spans="1:2">
       <c r="A73" t="s">
         <v>142</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B73" s="3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="15">
+    <row r="74" spans="1:2">
       <c r="A74" t="s">
         <v>143</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B74" s="3" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="15">
+    <row r="75" spans="1:2" ht="30">
       <c r="A75" t="s">
         <v>145</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B75" s="3" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="15">
+    <row r="76" spans="1:2">
       <c r="A76" t="s">
         <v>147</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B76" s="3" t="s">
         <v>148</v>
       </c>
     </row>

</xml_diff>